<commit_message>
Guest renamed to Participant
</commit_message>
<xml_diff>
--- a/scripts/Roster.xlsx
+++ b/scripts/Roster.xlsx
@@ -358,9 +358,6 @@
     <t>Ilana</t>
   </si>
   <si>
-    <t>Guest</t>
-  </si>
-  <si>
     <t>Piglanski</t>
   </si>
   <si>
@@ -424,9 +421,6 @@
     <t>gender</t>
   </si>
   <si>
-    <t>participant</t>
-  </si>
-  <si>
     <t>role</t>
   </si>
   <si>
@@ -461,6 +455,12 @@
   </si>
   <si>
     <t>612-616-3296</t>
+  </si>
+  <si>
+    <t>visitor</t>
+  </si>
+  <si>
+    <t>local</t>
   </si>
 </sst>
 </file>
@@ -866,8 +866,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51:IV51"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="F42" sqref="F42:F50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="11.25"/>
@@ -881,22 +881,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>134</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -916,7 +916,7 @@
         <v>3</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -936,7 +936,7 @@
         <v>7</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -956,7 +956,7 @@
         <v>10</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -976,7 +976,7 @@
         <v>14</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -996,7 +996,7 @@
         <v>19</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1016,7 +1016,7 @@
         <v>17</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1036,7 +1036,7 @@
         <v>22</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -1056,7 +1056,7 @@
         <v>25</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1076,7 +1076,7 @@
         <v>28</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1096,7 +1096,7 @@
         <v>31</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1116,7 +1116,7 @@
         <v>34</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -1136,7 +1136,7 @@
         <v>37</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -1156,7 +1156,7 @@
         <v>42</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -1176,7 +1176,7 @@
         <v>40</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -1196,7 +1196,7 @@
         <v>44</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -1216,7 +1216,7 @@
         <v>47</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -1236,7 +1236,7 @@
         <v>50</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -1256,7 +1256,7 @@
         <v>53</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1276,7 +1276,7 @@
         <v>56</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1296,7 +1296,7 @@
         <v>60</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -1316,7 +1316,7 @@
         <v>62</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -1336,7 +1336,7 @@
         <v>65</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -1356,7 +1356,7 @@
         <v>68</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -1376,7 +1376,7 @@
         <v>71</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -1396,7 +1396,7 @@
         <v>74</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -1416,7 +1416,7 @@
         <v>77</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -1436,7 +1436,7 @@
         <v>80</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -1456,7 +1456,7 @@
         <v>82</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -1476,7 +1476,7 @@
         <v>85</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -1496,7 +1496,7 @@
         <v>87</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -1516,7 +1516,7 @@
         <v>89</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -1536,7 +1536,7 @@
         <v>91</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -1556,7 +1556,7 @@
         <v>94</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -1576,7 +1576,7 @@
         <v>97</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -1596,7 +1596,7 @@
         <v>98</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -1616,7 +1616,7 @@
         <v>102</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -1636,7 +1636,7 @@
         <v>104</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -1656,7 +1656,7 @@
         <v>107</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -1676,7 +1676,7 @@
         <v>111</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -1696,15 +1696,15 @@
         <v>109</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
     </row>
     <row r="42" spans="1:6">
       <c r="A42" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B42" s="3" t="s">
         <v>114</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>115</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>2</v>
@@ -1713,18 +1713,18 @@
         <v>33249</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>113</v>
+        <v>147</v>
       </c>
     </row>
     <row r="43" spans="1:6">
       <c r="A43" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B43" s="3" t="s">
         <v>116</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>117</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>13</v>
@@ -1733,18 +1733,18 @@
         <v>33250</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>113</v>
+        <v>147</v>
       </c>
     </row>
     <row r="44" spans="1:6">
       <c r="A44" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C44" s="3" t="s">
         <v>2</v>
@@ -1753,18 +1753,18 @@
         <v>33251</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>113</v>
+        <v>147</v>
       </c>
     </row>
     <row r="45" spans="1:6">
       <c r="A45" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C45" s="3" t="s">
         <v>2</v>
@@ -1773,18 +1773,18 @@
         <v>33252</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>113</v>
+        <v>147</v>
       </c>
     </row>
     <row r="46" spans="1:6">
       <c r="A46" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C46" s="3" t="s">
         <v>2</v>
@@ -1793,18 +1793,18 @@
         <v>33253</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>113</v>
+        <v>147</v>
       </c>
     </row>
     <row r="47" spans="1:6">
       <c r="A47" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B47" s="3" t="s">
         <v>121</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>122</v>
       </c>
       <c r="C47" s="3" t="s">
         <v>13</v>
@@ -1813,18 +1813,18 @@
         <v>33254</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>113</v>
+        <v>147</v>
       </c>
     </row>
     <row r="48" spans="1:6">
       <c r="A48" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C48" s="3" t="s">
         <v>13</v>
@@ -1833,18 +1833,18 @@
         <v>33255</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>113</v>
+        <v>147</v>
       </c>
     </row>
     <row r="49" spans="1:6">
       <c r="A49" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>2</v>
@@ -1853,18 +1853,18 @@
         <v>33256</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>113</v>
+        <v>147</v>
       </c>
     </row>
     <row r="50" spans="1:6">
       <c r="A50" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C50" s="3" t="s">
         <v>2</v>
@@ -1873,10 +1873,10 @@
         <v>33257</v>
       </c>
       <c r="E50" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="F50" s="3" t="s">
         <v>147</v>
-      </c>
-      <c r="F50" s="3" t="s">
-        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed nickName Roster file
</commit_message>
<xml_diff>
--- a/scripts/Roster.xlsx
+++ b/scripts/Roster.xlsx
@@ -463,7 +463,7 @@
     <t>local</t>
   </si>
   <si>
-    <t>Nikki</t>
+    <t>nickName</t>
   </si>
 </sst>
 </file>
@@ -869,8 +869,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="11.25"/>

</xml_diff>

<commit_message>
seedDB gender to lower case
</commit_message>
<xml_diff>
--- a/scripts/Roster.xlsx
+++ b/scripts/Roster.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="225">
   <si>
     <t>email</t>
   </si>
@@ -653,6 +653,45 @@
   </si>
   <si>
     <t>birthday</t>
+  </si>
+  <si>
+    <t>612-616-3288</t>
+  </si>
+  <si>
+    <t>612-616-3289</t>
+  </si>
+  <si>
+    <t>612-616-3290</t>
+  </si>
+  <si>
+    <t>612-616-3291</t>
+  </si>
+  <si>
+    <t>612-616-3292</t>
+  </si>
+  <si>
+    <t>612-616-3293</t>
+  </si>
+  <si>
+    <t>612-616-3294</t>
+  </si>
+  <si>
+    <t>612-616-3295</t>
+  </si>
+  <si>
+    <t>612-616-3296</t>
+  </si>
+  <si>
+    <t>612-616-3297</t>
+  </si>
+  <si>
+    <t>612-616-3298</t>
+  </si>
+  <si>
+    <t>612-616-3299</t>
+  </si>
+  <si>
+    <t>612-616-3300</t>
   </si>
 </sst>
 </file>
@@ -1078,8 +1117,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="76" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="76" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="F41" sqref="F41:F54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
@@ -2193,6 +2232,9 @@
       <c r="E42" s="4">
         <v>33583</v>
       </c>
+      <c r="F42" s="3" t="s">
+        <v>212</v>
+      </c>
       <c r="G42" s="3" t="s">
         <v>173</v>
       </c>
@@ -2216,6 +2258,9 @@
       <c r="E43" s="4">
         <v>33281</v>
       </c>
+      <c r="F43" s="3" t="s">
+        <v>213</v>
+      </c>
       <c r="G43" s="3" t="s">
         <v>173</v>
       </c>
@@ -2239,6 +2284,9 @@
       <c r="E44" s="4">
         <v>33402</v>
       </c>
+      <c r="F44" s="3" t="s">
+        <v>214</v>
+      </c>
       <c r="G44" s="3" t="s">
         <v>173</v>
       </c>
@@ -2262,6 +2310,9 @@
       <c r="E45" s="4">
         <v>33464</v>
       </c>
+      <c r="F45" s="3" t="s">
+        <v>215</v>
+      </c>
       <c r="G45" s="3" t="s">
         <v>173</v>
       </c>
@@ -2285,6 +2336,9 @@
       <c r="E46" s="4">
         <v>33434</v>
       </c>
+      <c r="F46" s="3" t="s">
+        <v>216</v>
+      </c>
       <c r="G46" s="3" t="s">
         <v>173</v>
       </c>
@@ -2308,6 +2362,9 @@
       <c r="E47" s="4">
         <v>33497</v>
       </c>
+      <c r="F47" s="3" t="s">
+        <v>217</v>
+      </c>
       <c r="G47" s="3" t="s">
         <v>173</v>
       </c>
@@ -2331,6 +2388,9 @@
       <c r="E48" s="4">
         <v>33528</v>
       </c>
+      <c r="F48" s="3" t="s">
+        <v>218</v>
+      </c>
       <c r="G48" s="3" t="s">
         <v>173</v>
       </c>
@@ -2354,6 +2414,9 @@
       <c r="E49" s="4">
         <v>33346</v>
       </c>
+      <c r="F49" s="3" t="s">
+        <v>219</v>
+      </c>
       <c r="G49" s="3" t="s">
         <v>173</v>
       </c>
@@ -2377,6 +2440,9 @@
       <c r="E50" s="4">
         <v>33561</v>
       </c>
+      <c r="F50" s="3" t="s">
+        <v>220</v>
+      </c>
       <c r="G50" s="3" t="s">
         <v>173</v>
       </c>
@@ -2400,6 +2466,9 @@
       <c r="E51" s="4">
         <v>30267</v>
       </c>
+      <c r="F51" s="3" t="s">
+        <v>221</v>
+      </c>
       <c r="G51" s="3" t="s">
         <v>179</v>
       </c>
@@ -2423,6 +2492,9 @@
       <c r="E52" s="4">
         <v>25431</v>
       </c>
+      <c r="F52" s="3" t="s">
+        <v>222</v>
+      </c>
       <c r="G52" s="3" t="s">
         <v>179</v>
       </c>
@@ -2446,6 +2518,9 @@
       <c r="E53" s="4">
         <v>30073</v>
       </c>
+      <c r="F53" s="3" t="s">
+        <v>223</v>
+      </c>
       <c r="G53" s="3" t="s">
         <v>179</v>
       </c>
@@ -2468,6 +2543,9 @@
       </c>
       <c r="E54" s="4">
         <v>27800</v>
+      </c>
+      <c r="F54" s="3" t="s">
+        <v>224</v>
       </c>
       <c r="G54" s="3" t="s">
         <v>179</v>

</xml_diff>